<commit_message>
Added hasGameName policy, with test in policyTest.js, and applied it to gameController.create
</commit_message>
<xml_diff>
--- a/policyOverview.xlsx
+++ b/policyOverview.xlsx
@@ -523,7 +523,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +617,7 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="3" t="s">

</xml_diff>

<commit_message>
Added policy for hasPassword, with corresponding test. Does not yet validate password for content
</commit_message>
<xml_diff>
--- a/policyOverview.xlsx
+++ b/policyOverview.xlsx
@@ -523,7 +523,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
@@ -606,7 +606,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">

</xml_diff>